<commit_message>
add relationship handle in FileController
</commit_message>
<xml_diff>
--- a/Excel/Relationships.xlsx
+++ b/Excel/Relationships.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Giapha\Genealogy.Server\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1963A13-0B6E-4AD8-AF20-69D51FC2D322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,52 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>MainMemId</t>
+  </si>
+  <si>
+    <t>SubMemId</t>
+  </si>
+  <si>
+    <t>RelateCode</t>
+  </si>
+  <si>
+    <t>DateStart</t>
+  </si>
+  <si>
+    <t>0054042f-4d37-4800-a8ed-7ad25e23b764</t>
+  </si>
+  <si>
+    <t>13b2f73c-65f2-4c1a-baa8-00e9cd5b18ac</t>
+  </si>
+  <si>
+    <t>1a719c1b-8b56-42eb-adf2-4e40681d8806</t>
+  </si>
+  <si>
+    <t>2d4bf196-a96a-47ed-a64a-f5f9c95be937</t>
+  </si>
+  <si>
+    <t>58d017d5-ef0c-4ea0-ae95-b8e50fa37b6d</t>
+  </si>
+  <si>
+    <t>812527b5-2a2e-42bc-b5dd-9211bb750987</t>
+  </si>
+  <si>
+    <t>c51a1ee3-aedf-4215-bb24-e23f332e4749</t>
+  </si>
+  <si>
+    <t>d93088c1-9f47-4034-897f-10fdec8c5700</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +380,192 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>